<commit_message>
Add source for the table
</commit_message>
<xml_diff>
--- a/references/Pop_stats.xlsx
+++ b/references/Pop_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\LU-python-course-project-2025\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB9727F-C130-4E86-A12C-26F22B2B3CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DD7FB5-F154-49C2-A854-0FBB1C701090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F672C57-36C1-466A-ACC0-07BE7FC92B00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6F672C57-36C1-466A-ACC0-07BE7FC92B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Recommended provinces" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="157">
   <si>
     <t>City/Province</t>
   </si>
@@ -505,6 +505,9 @@
   </si>
   <si>
     <t>Lund (Zviedrija)</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/europe/comments/4kdvo1/the_thirty_largest_cities_in_europe_by_population/#lightbox</t>
   </si>
 </sst>
 </file>
@@ -673,15 +676,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>357927</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>96523</xdr:rowOff>
+      <xdr:colOff>557952</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>153673</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>570941</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>86998</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>161366</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144148</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -710,7 +713,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10540152" y="96523"/>
+          <a:off x="10740177" y="344173"/>
           <a:ext cx="7528214" cy="5133975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1042,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15E336A-67D8-4AB6-AA9B-A495956018A1}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -1970,9 +1973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66176A7-21DE-4132-A487-5D3F9EEA404F}">
   <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,7 +2192,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2228,7 +2231,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2250,7 +2253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>82</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>70</v>
       </c>
@@ -2350,7 +2353,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>74</v>
       </c>
@@ -2360,8 +2363,11 @@
       <c r="C30" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O30" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>137</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>